<commit_message>
Timesheet & Reformatted Excel Import code and spreadsheet
You should be able to click "import" in the admin tool and select the
included "test.xlsx" file, and the contents of that file will be added
to our online database.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\SeniorProject2015\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7905" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="test_registrants" sheetId="1" r:id="rId1"/>
-    <sheet name="test_students" sheetId="2" r:id="rId2"/>
-    <sheet name="test_employees" sheetId="3" r:id="rId3"/>
+    <sheet name="registrant" sheetId="1" r:id="rId1"/>
+    <sheet name="student" sheetId="2" r:id="rId2"/>
+    <sheet name="employee" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,49 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>businessname</t>
-  </si>
-  <si>
-    <t>jobtitle</t>
-  </si>
-  <si>
-    <t>fname</t>
-  </si>
-  <si>
-    <t>lname</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>studentid</t>
-  </si>
-  <si>
-    <t>college</t>
-  </si>
-  <si>
-    <t>major</t>
-  </si>
-  <si>
-    <t>gyear</t>
-  </si>
-  <si>
-    <t>standing</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>John</t>
   </si>
@@ -79,18 +37,9 @@
     <t>who@hotmail.com</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>Student</t>
   </si>
   <si>
-    <t>Employer</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>where@gmail.com</t>
   </si>
   <si>
@@ -100,15 +49,9 @@
     <t>Darcy</t>
   </si>
   <si>
-    <t>EWU</t>
-  </si>
-  <si>
     <t>Computer Science</t>
   </si>
   <si>
-    <t>Sophomore</t>
-  </si>
-  <si>
     <t>Home Tome</t>
   </si>
   <si>
@@ -139,10 +82,73 @@
     <t>skcreg93@gitgud.com</t>
   </si>
   <si>
-    <t>WSU</t>
-  </si>
-  <si>
     <t>Freshman</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Fname</t>
+  </si>
+  <si>
+    <t>Lname</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Registered</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>RegType</t>
+  </si>
+  <si>
+    <t>Graduation</t>
+  </si>
+  <si>
+    <t>StudentID</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>College</t>
+  </si>
+  <si>
+    <t>ClassStanding</t>
+  </si>
+  <si>
+    <t>Alumnus</t>
+  </si>
+  <si>
+    <t>Eastern Washington University</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Job</t>
   </si>
 </sst>
 </file>
@@ -187,9 +193,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -539,138 +546,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>123456</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>15098889999</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="H2" s="2">
+        <v>42139.683877314812</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>987654</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="D3">
         <v>19992224444</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="H3" s="2">
+        <v>42139.685208333336</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>567438</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4">
+        <v>13</v>
+      </c>
+      <c r="D4">
         <v>12223334444</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="H4" s="2">
+        <v>42139.646921296298</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>889912</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5">
+        <v>16</v>
+      </c>
+      <c r="D5">
         <v>19871231234</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="H5" s="2">
+        <v>42139.687581018516</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -680,30 +721,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -711,19 +759,19 @@
         <v>123456</v>
       </c>
       <c r="B2">
-        <v>876</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
+        <v>2016</v>
+      </c>
+      <c r="C2">
+        <v>1234567890</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2">
-        <v>2016</v>
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -731,19 +779,19 @@
         <v>889912</v>
       </c>
       <c r="B3">
-        <v>384</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
+        <v>2018</v>
+      </c>
+      <c r="C3">
+        <v>1112223334</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3">
-        <v>2018</v>
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -755,24 +803,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -780,10 +830,10 @@
         <v>987654</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -791,10 +841,10 @@
         <v>567438</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>